<commit_message>
Cập nhật hồ sơ ngoài excel template và theo dõi suất ăn
</commit_message>
<xml_diff>
--- a/QUANGHANH2/excel/TCLD/Hoso/ho-so-ngoai.xlsx
+++ b/QUANGHANH2/excel/TCLD/Hoso/ho-so-ngoai.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nguye\Desktop\project merge\QUANGHANH-PROTOTYPE\QUANGHANH2\excel\TCLD\Hoso\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nguye\Desktop\Project\QUANGHANH-PROTOTYPE\QUANGHANH2\excel\TCLD\Hoso\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C188DDEC-BC33-40A9-BDDE-E2AD4C1AF114}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78776CA3-C2A6-4597-BCAF-38EABDC35B4C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="4455" windowWidth="20730" windowHeight="11160" xr2:uid="{E6707C89-2A6A-4A0F-B365-0A2970733FDD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E6707C89-2A6A-4A0F-B365-0A2970733FDD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,37 +30,73 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="20">
   <si>
     <t>STT</t>
   </si>
   <si>
-    <t>Số thẻ</t>
-  </si>
-  <si>
     <t>Họ và tên</t>
   </si>
   <si>
-    <t>ĐV khi CDHĐ</t>
-  </si>
-  <si>
     <t>Số BHXH</t>
   </si>
   <si>
-    <t>Số Điện Thoại</t>
-  </si>
-  <si>
     <t>Địa chỉ</t>
   </si>
   <si>
     <t>Loại chấm dứt</t>
+  </si>
+  <si>
+    <t>Mã nhân viên</t>
+  </si>
+  <si>
+    <t>Đơn vị khi CDHĐ</t>
+  </si>
+  <si>
+    <t>Số điện thoại</t>
+  </si>
+  <si>
+    <t>Giấy tờ</t>
+  </si>
+  <si>
+    <t>Tên</t>
+  </si>
+  <si>
+    <t>Kiểu</t>
+  </si>
+  <si>
+    <t>Ngày trả</t>
+  </si>
+  <si>
+    <t>Ngày cấp</t>
+  </si>
+  <si>
+    <t>Chứng chỉ</t>
+  </si>
+  <si>
+    <t>Bằng cấp</t>
+  </si>
+  <si>
+    <t>Thông tin người ủy quyền lấy hồ sơ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tên </t>
+  </si>
+  <si>
+    <t>Quan hệ</t>
+  </si>
+  <si>
+    <t>Số CMT</t>
+  </si>
+  <si>
+    <t>HỒ SƠ NGOÀI</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -68,16 +104,35 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -85,12 +140,38 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -405,46 +486,194 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5C66C84-202B-4DD4-B088-EB1F19DF37CD}">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:X3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="15.28515625" customWidth="1"/>
-    <col min="6" max="6" width="18.140625" customWidth="1"/>
-    <col min="8" max="8" width="15.7109375" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="21.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="27.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="20.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="23" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.140625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="21.5703125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="32.85546875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="21.140625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="17.42578125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="16.5703125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="17.28515625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="16.85546875" style="1" customWidth="1"/>
+    <col min="17" max="17" width="17.140625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="16" style="1" customWidth="1"/>
+    <col min="19" max="19" width="22.5703125" style="1" customWidth="1"/>
+    <col min="20" max="20" width="20.5703125" style="1" customWidth="1"/>
+    <col min="21" max="21" width="16.7109375" style="1" customWidth="1"/>
+    <col min="22" max="22" width="24" style="1" customWidth="1"/>
+    <col min="23" max="23" width="22.42578125" style="1" customWidth="1"/>
+    <col min="24" max="24" width="20.5703125" style="1" customWidth="1"/>
+    <col min="25" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:24" s="3" customFormat="1" ht="22.5" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
+      <c r="X1" s="2"/>
+    </row>
+    <row r="2" spans="1:24" s="3" customFormat="1" ht="22.5" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="I2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="R2" s="4"/>
+      <c r="S2" s="4"/>
+      <c r="T2" s="4"/>
+      <c r="U2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="V2" s="4"/>
+      <c r="W2" s="4"/>
+      <c r="X2" s="4"/>
+    </row>
+    <row r="3" spans="1:24" s="3" customFormat="1" ht="22.5" x14ac:dyDescent="0.3">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="N3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="O3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="P3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="R3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="S3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="T3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="U3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="V3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="W3" s="5" t="s">
         <v>7</v>
+      </c>
+      <c r="X3" s="5" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="13">
+    <mergeCell ref="A1:X1"/>
+    <mergeCell ref="U2:X2"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="I2:L2"/>
+    <mergeCell ref="M2:P2"/>
+    <mergeCell ref="Q2:T2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Cập nhật màn hình tổng nhân lực và cập nhật paging
</commit_message>
<xml_diff>
--- a/QUANGHANH2/excel/TCLD/Hoso/ho-so-ngoai.xlsx
+++ b/QUANGHANH2/excel/TCLD/Hoso/ho-so-ngoai.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nguye\Desktop\Project\QUANGHANH-PROTOTYPE\QUANGHANH2\excel\TCLD\Hoso\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nguye\Desktop\project merge\QUANGHANH-PROTOTYPE\QUANGHANH2\excel\TCLD\Hoso\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78776CA3-C2A6-4597-BCAF-38EABDC35B4C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C188DDEC-BC33-40A9-BDDE-E2AD4C1AF114}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E6707C89-2A6A-4A0F-B365-0A2970733FDD}"/>
+    <workbookView xWindow="28680" yWindow="4455" windowWidth="20730" windowHeight="11160" xr2:uid="{E6707C89-2A6A-4A0F-B365-0A2970733FDD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,73 +30,37 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>STT</t>
   </si>
   <si>
+    <t>Số thẻ</t>
+  </si>
+  <si>
     <t>Họ và tên</t>
   </si>
   <si>
+    <t>ĐV khi CDHĐ</t>
+  </si>
+  <si>
     <t>Số BHXH</t>
   </si>
   <si>
+    <t>Số Điện Thoại</t>
+  </si>
+  <si>
     <t>Địa chỉ</t>
   </si>
   <si>
     <t>Loại chấm dứt</t>
-  </si>
-  <si>
-    <t>Mã nhân viên</t>
-  </si>
-  <si>
-    <t>Đơn vị khi CDHĐ</t>
-  </si>
-  <si>
-    <t>Số điện thoại</t>
-  </si>
-  <si>
-    <t>Giấy tờ</t>
-  </si>
-  <si>
-    <t>Tên</t>
-  </si>
-  <si>
-    <t>Kiểu</t>
-  </si>
-  <si>
-    <t>Ngày trả</t>
-  </si>
-  <si>
-    <t>Ngày cấp</t>
-  </si>
-  <si>
-    <t>Chứng chỉ</t>
-  </si>
-  <si>
-    <t>Bằng cấp</t>
-  </si>
-  <si>
-    <t>Thông tin người ủy quyền lấy hồ sơ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tên </t>
-  </si>
-  <si>
-    <t>Quan hệ</t>
-  </si>
-  <si>
-    <t>Số CMT</t>
-  </si>
-  <si>
-    <t>HỒ SƠ NGOÀI</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -104,35 +68,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -140,38 +85,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -486,194 +405,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5C66C84-202B-4DD4-B088-EB1F19DF37CD}">
-  <dimension ref="A1:X3"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="21.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="27.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.5703125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="20.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="23" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="27.140625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="21.5703125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="32.85546875" style="1" customWidth="1"/>
-    <col min="12" max="12" width="21.140625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="17.42578125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="16.5703125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="17.28515625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="16.85546875" style="1" customWidth="1"/>
-    <col min="17" max="17" width="17.140625" style="1" customWidth="1"/>
-    <col min="18" max="18" width="16" style="1" customWidth="1"/>
-    <col min="19" max="19" width="22.5703125" style="1" customWidth="1"/>
-    <col min="20" max="20" width="20.5703125" style="1" customWidth="1"/>
-    <col min="21" max="21" width="16.7109375" style="1" customWidth="1"/>
-    <col min="22" max="22" width="24" style="1" customWidth="1"/>
-    <col min="23" max="23" width="22.42578125" style="1" customWidth="1"/>
-    <col min="24" max="24" width="20.5703125" style="1" customWidth="1"/>
-    <col min="25" max="16384" width="9.140625" style="1"/>
+    <col min="4" max="4" width="15.28515625" customWidth="1"/>
+    <col min="6" max="6" width="18.140625" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="3" customFormat="1" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2"/>
-      <c r="W1" s="2"/>
-      <c r="X1" s="2"/>
-    </row>
-    <row r="2" spans="1:24" s="3" customFormat="1" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="4" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" s="4" t="s">
+      <c r="H1" t="s">
         <v>7</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="R2" s="4"/>
-      <c r="S2" s="4"/>
-      <c r="T2" s="4"/>
-      <c r="U2" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="V2" s="4"/>
-      <c r="W2" s="4"/>
-      <c r="X2" s="4"/>
-    </row>
-    <row r="3" spans="1:24" s="3" customFormat="1" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="K3" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="L3" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="M3" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="N3" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="O3" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="P3" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q3" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="R3" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="S3" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="T3" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="U3" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="V3" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="W3" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="X3" s="5" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="A1:X1"/>
-    <mergeCell ref="U2:X2"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="I2:L2"/>
-    <mergeCell ref="M2:P2"/>
-    <mergeCell ref="Q2:T2"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update file excel cho ho so ngoai va suat an
</commit_message>
<xml_diff>
--- a/QUANGHANH2/excel/TCLD/Hoso/ho-so-ngoai.xlsx
+++ b/QUANGHANH2/excel/TCLD/Hoso/ho-so-ngoai.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nguye\Desktop\project merge\QUANGHANH-PROTOTYPE\QUANGHANH2\excel\TCLD\Hoso\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nguye\Desktop\Project\QUANGHANH-PROTOTYPE\QUANGHANH2\excel\TCLD\Hoso\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C188DDEC-BC33-40A9-BDDE-E2AD4C1AF114}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78776CA3-C2A6-4597-BCAF-38EABDC35B4C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="4455" windowWidth="20730" windowHeight="11160" xr2:uid="{E6707C89-2A6A-4A0F-B365-0A2970733FDD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E6707C89-2A6A-4A0F-B365-0A2970733FDD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,37 +30,73 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="20">
   <si>
     <t>STT</t>
   </si>
   <si>
-    <t>Số thẻ</t>
-  </si>
-  <si>
     <t>Họ và tên</t>
   </si>
   <si>
-    <t>ĐV khi CDHĐ</t>
-  </si>
-  <si>
     <t>Số BHXH</t>
   </si>
   <si>
-    <t>Số Điện Thoại</t>
-  </si>
-  <si>
     <t>Địa chỉ</t>
   </si>
   <si>
     <t>Loại chấm dứt</t>
+  </si>
+  <si>
+    <t>Mã nhân viên</t>
+  </si>
+  <si>
+    <t>Đơn vị khi CDHĐ</t>
+  </si>
+  <si>
+    <t>Số điện thoại</t>
+  </si>
+  <si>
+    <t>Giấy tờ</t>
+  </si>
+  <si>
+    <t>Tên</t>
+  </si>
+  <si>
+    <t>Kiểu</t>
+  </si>
+  <si>
+    <t>Ngày trả</t>
+  </si>
+  <si>
+    <t>Ngày cấp</t>
+  </si>
+  <si>
+    <t>Chứng chỉ</t>
+  </si>
+  <si>
+    <t>Bằng cấp</t>
+  </si>
+  <si>
+    <t>Thông tin người ủy quyền lấy hồ sơ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tên </t>
+  </si>
+  <si>
+    <t>Quan hệ</t>
+  </si>
+  <si>
+    <t>Số CMT</t>
+  </si>
+  <si>
+    <t>HỒ SƠ NGOÀI</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -68,16 +104,35 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -85,12 +140,38 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -405,46 +486,194 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5C66C84-202B-4DD4-B088-EB1F19DF37CD}">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:X3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="15.28515625" customWidth="1"/>
-    <col min="6" max="6" width="18.140625" customWidth="1"/>
-    <col min="8" max="8" width="15.7109375" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="21.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="27.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="20.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="23" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.140625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="21.5703125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="32.85546875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="21.140625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="17.42578125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="16.5703125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="17.28515625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="16.85546875" style="1" customWidth="1"/>
+    <col min="17" max="17" width="17.140625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="16" style="1" customWidth="1"/>
+    <col min="19" max="19" width="22.5703125" style="1" customWidth="1"/>
+    <col min="20" max="20" width="20.5703125" style="1" customWidth="1"/>
+    <col min="21" max="21" width="16.7109375" style="1" customWidth="1"/>
+    <col min="22" max="22" width="24" style="1" customWidth="1"/>
+    <col min="23" max="23" width="22.42578125" style="1" customWidth="1"/>
+    <col min="24" max="24" width="20.5703125" style="1" customWidth="1"/>
+    <col min="25" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:24" s="3" customFormat="1" ht="22.5" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
+      <c r="X1" s="2"/>
+    </row>
+    <row r="2" spans="1:24" s="3" customFormat="1" ht="22.5" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="I2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="R2" s="4"/>
+      <c r="S2" s="4"/>
+      <c r="T2" s="4"/>
+      <c r="U2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="V2" s="4"/>
+      <c r="W2" s="4"/>
+      <c r="X2" s="4"/>
+    </row>
+    <row r="3" spans="1:24" s="3" customFormat="1" ht="22.5" x14ac:dyDescent="0.3">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="N3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="O3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="P3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="R3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="S3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="T3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="U3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="V3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="W3" s="5" t="s">
         <v>7</v>
+      </c>
+      <c r="X3" s="5" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="13">
+    <mergeCell ref="A1:X1"/>
+    <mergeCell ref="U2:X2"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="I2:L2"/>
+    <mergeCell ref="M2:P2"/>
+    <mergeCell ref="Q2:T2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>